<commit_message>
correct the arguments and fields for static tract data
</commit_message>
<xml_diff>
--- a/data/BlockDataDefinition.xlsx
+++ b/data/BlockDataDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/38032999/softwares/dataArts/cdp-proc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000524DE-F7A4-634D-B0D1-B441EB5EFBFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3712A619-8951-B74C-8451-25D562D79193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="2320" windowWidth="22200" windowHeight="14260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11300" yWindow="3400" windowWidth="22200" windowHeight="14260" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AllBlockVariables" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="375">
   <si>
     <t>Id</t>
   </si>
@@ -1118,9 +1118,6 @@
     <t>ACSKey</t>
   </si>
   <si>
-    <t>GEO_ID</t>
-  </si>
-  <si>
     <t>STATE</t>
   </si>
   <si>
@@ -3479,10 +3476,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3505,13 +3502,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="C2" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -3541,7 +3538,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>366</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>369</v>
@@ -3549,390 +3546,378 @@
       <c r="C5" t="s">
         <v>373</v>
       </c>
-      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>370</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>374</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C36" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C38" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C39" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B40" t="s">
-        <v>113</v>
-      </c>
-      <c r="C40" t="s">
         <v>277</v>
       </c>
     </row>
@@ -3944,10 +3929,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3971,13 +3956,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="C2" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -4007,7 +3992,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>366</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>369</v>
@@ -4015,38 +4000,26 @@
       <c r="C5" t="s">
         <v>373</v>
       </c>
-      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>370</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>374</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" t="s">
         <v>279</v>
       </c>
     </row>
@@ -4057,10 +4030,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J16348"/>
+  <dimension ref="A1:J16347"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4083,13 +4056,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="C2" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -4119,7 +4092,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>366</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>369</v>
@@ -4127,150 +4100,141 @@
       <c r="C5" t="s">
         <v>373</v>
       </c>
-      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>370</v>
-      </c>
-      <c r="C6" t="s">
-        <v>374</v>
+        <v>49</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>291</v>
-      </c>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C19" s="5"/>
@@ -4459,7 +4423,7 @@
       <c r="C80" s="5"/>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C81" s="5"/>
+      <c r="C81" s="1"/>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C82" s="1"/>
@@ -53258,9 +53222,6 @@
     </row>
     <row r="16347" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C16347" s="1"/>
-    </row>
-    <row r="16348" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C16348" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
@@ -53271,10 +53232,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:XFD6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53298,13 +53259,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="C2" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -53334,7 +53295,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>366</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>369</v>
@@ -53342,82 +53303,70 @@
       <c r="C5" t="s">
         <v>373</v>
       </c>
-      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>370</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>374</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" t="s">
         <v>297</v>
       </c>
     </row>
@@ -53428,10 +53377,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:XFD6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53454,13 +53403,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="C2" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -53490,7 +53439,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>366</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>369</v>
@@ -53498,192 +53447,180 @@
       <c r="C5" t="s">
         <v>373</v>
       </c>
-      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>370</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>374</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C12" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>374</v>
       </c>
       <c r="C14" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
-        <v>375</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C16" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C17" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C18" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C20" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B21" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C21" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>154</v>
-      </c>
-      <c r="B22" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" t="s">
         <v>313</v>
       </c>
     </row>
@@ -53694,10 +53631,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:XFD6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53721,13 +53658,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="C2" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -53757,7 +53694,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>366</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>369</v>
@@ -53765,302 +53702,290 @@
       <c r="C5" t="s">
         <v>373</v>
       </c>
-      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>370</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>374</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>159</v>
       </c>
       <c r="C8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C9" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C10" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C11" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C12" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C13" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C14" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C15" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C16" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C17" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B18" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C18" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C19" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B20" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C20" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B21" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C21" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B22" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C22" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C23" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B24" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C24" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B25" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C25" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B26" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C26" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B27" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C27" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B28" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C28" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B29" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C29" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B30" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C30" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B31" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C31" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>204</v>
-      </c>
-      <c r="B32" t="s">
-        <v>205</v>
-      </c>
-      <c r="C32" t="s">
         <v>339</v>
       </c>
     </row>
@@ -54071,10 +53996,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -54096,13 +54021,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="C2" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -54132,7 +54057,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>366</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>369</v>
@@ -54140,236 +54065,224 @@
       <c r="C5" t="s">
         <v>373</v>
       </c>
-      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>370</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>374</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>206</v>
       </c>
       <c r="C8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C10" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C11" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C13" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C14" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C15" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C16" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C17" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>216</v>
       </c>
       <c r="B18" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C18" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B19" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>218</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C20" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C21" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>222</v>
       </c>
       <c r="B22" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C22" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B23" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C23" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B24" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C24" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B25" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C25" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>228</v>
-      </c>
-      <c r="B26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C26" t="s">
         <v>359</v>
       </c>
     </row>

</xml_diff>